<commit_message>
🐛 fix carroyage position + square size
</commit_message>
<xml_diff>
--- a/carroyage.xlsx
+++ b/carroyage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="566">
   <si>
     <t xml:space="preserve">.</t>
   </si>
@@ -1827,16 +1827,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM53"/>
+  <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="1" style="0" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="1" style="0" width="5.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,6 +1956,9 @@
       <c r="AM1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -2076,6 +2078,9 @@
       <c r="AM2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN2" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -2195,6 +2200,9 @@
       <c r="AM3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2314,6 +2322,9 @@
       <c r="AM4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN4" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2433,6 +2444,9 @@
       <c r="AM5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN5" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2552,6 +2566,9 @@
       <c r="AM6" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN6" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -2671,6 +2688,9 @@
       <c r="AM7" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN7" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -2790,6 +2810,9 @@
       <c r="AM8" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN8" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -2909,6 +2932,9 @@
       <c r="AM9" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN9" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -3028,6 +3054,9 @@
       <c r="AM10" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN10" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -3040,41 +3069,41 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P11" s="1" t="s">
         <v>0</v>
       </c>
@@ -3145,6 +3174,9 @@
         <v>0</v>
       </c>
       <c r="AM11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3159,41 +3191,41 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P12" s="1" t="s">
         <v>0</v>
       </c>
@@ -3264,6 +3296,9 @@
         <v>0</v>
       </c>
       <c r="AM12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3278,41 +3313,41 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P13" s="1" t="s">
         <v>0</v>
       </c>
@@ -3383,6 +3418,9 @@
         <v>0</v>
       </c>
       <c r="AM13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3397,41 +3435,41 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P14" s="1" t="s">
         <v>0</v>
       </c>
@@ -3502,6 +3540,9 @@
         <v>0</v>
       </c>
       <c r="AM14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3522,35 +3563,35 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P15" s="1" t="s">
         <v>0</v>
       </c>
@@ -3621,6 +3662,9 @@
         <v>0</v>
       </c>
       <c r="AM15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3641,32 +3685,32 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="O16" s="1" t="s">
         <v>0</v>
       </c>
@@ -3740,6 +3784,9 @@
         <v>0</v>
       </c>
       <c r="AM16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3760,32 +3807,32 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="O17" s="1" t="s">
         <v>0</v>
       </c>
@@ -3859,6 +3906,9 @@
         <v>0</v>
       </c>
       <c r="AM17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3879,32 +3929,32 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="O18" s="1" t="s">
         <v>0</v>
       </c>
@@ -3978,6 +4028,9 @@
         <v>0</v>
       </c>
       <c r="AM18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3998,32 +4051,32 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="O19" s="1" t="s">
         <v>0</v>
       </c>
@@ -4097,6 +4150,9 @@
         <v>0</v>
       </c>
       <c r="AM19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4117,32 +4173,32 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="O20" s="1" t="s">
         <v>0</v>
       </c>
@@ -4216,6 +4272,9 @@
         <v>0</v>
       </c>
       <c r="AM20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4239,32 +4298,32 @@
         <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P21" s="1" t="s">
         <v>0</v>
       </c>
@@ -4335,6 +4394,9 @@
         <v>0</v>
       </c>
       <c r="AM21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4358,32 +4420,32 @@
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P22" s="1" t="s">
         <v>0</v>
       </c>
@@ -4454,6 +4516,9 @@
         <v>0</v>
       </c>
       <c r="AM22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4477,32 +4542,32 @@
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P23" s="1" t="s">
         <v>0</v>
       </c>
@@ -4573,6 +4638,9 @@
         <v>0</v>
       </c>
       <c r="AM23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4596,32 +4664,32 @@
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P24" s="1" t="s">
         <v>0</v>
       </c>
@@ -4692,6 +4760,9 @@
         <v>0</v>
       </c>
       <c r="AM24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN24" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4715,32 +4786,32 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P25" s="1" t="s">
         <v>0</v>
       </c>
@@ -4811,6 +4882,9 @@
         <v>0</v>
       </c>
       <c r="AM25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4834,32 +4908,32 @@
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="P26" s="1" t="s">
         <v>0</v>
       </c>
@@ -4930,6 +5004,9 @@
         <v>0</v>
       </c>
       <c r="AM26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4950,77 +5027,77 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="S27" s="1" t="s">
+      <c r="T27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="T27" s="1" t="s">
+      <c r="U27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="U27" s="1" t="s">
+      <c r="V27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="V27" s="1" t="s">
+      <c r="W27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="X27" s="1" t="s">
+      <c r="Y27" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="Y27" s="1" t="s">
+      <c r="Z27" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="Z27" s="1" t="s">
+      <c r="AA27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AA27" s="1" t="s">
+      <c r="AB27" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AB27" s="1" t="s">
+      <c r="AC27" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="AC27" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD27" s="1" t="s">
         <v>0</v>
       </c>
@@ -5049,6 +5126,9 @@
         <v>0</v>
       </c>
       <c r="AM27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5069,77 +5149,77 @@
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="R28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="T28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="U28" s="1" t="s">
+      <c r="V28" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="W28" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="X28" s="1" t="s">
+      <c r="Y28" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="Y28" s="1" t="s">
+      <c r="Z28" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Z28" s="1" t="s">
+      <c r="AA28" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AA28" s="1" t="s">
+      <c r="AB28" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AC28" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AC28" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD28" s="1" t="s">
         <v>0</v>
       </c>
@@ -5168,6 +5248,9 @@
         <v>0</v>
       </c>
       <c r="AM28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5188,77 +5271,77 @@
         <v>0</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="T29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="U29" s="1" t="s">
+      <c r="V29" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="V29" s="1" t="s">
+      <c r="W29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="X29" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="X29" s="1" t="s">
+      <c r="Y29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Y29" s="1" t="s">
+      <c r="Z29" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="Z29" s="1" t="s">
+      <c r="AA29" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AA29" s="1" t="s">
+      <c r="AB29" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AC29" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="AC29" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD29" s="1" t="s">
         <v>0</v>
       </c>
@@ -5287,6 +5370,9 @@
         <v>0</v>
       </c>
       <c r="AM29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN29" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5307,77 +5393,77 @@
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="R30" s="1" t="s">
+      <c r="S30" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="T30" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="T30" s="1" t="s">
+      <c r="U30" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="U30" s="1" t="s">
+      <c r="V30" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="V30" s="1" t="s">
+      <c r="W30" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="X30" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="X30" s="1" t="s">
+      <c r="Y30" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="Y30" s="1" t="s">
+      <c r="Z30" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Z30" s="1" t="s">
+      <c r="AA30" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="AA30" s="1" t="s">
+      <c r="AB30" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="AB30" s="1" t="s">
+      <c r="AC30" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="AC30" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD30" s="1" t="s">
         <v>0</v>
       </c>
@@ -5406,6 +5492,9 @@
         <v>0</v>
       </c>
       <c r="AM30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5426,77 +5515,77 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="S31" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="T31" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="T31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="U31" s="1" t="s">
+      <c r="V31" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="V31" s="1" t="s">
+      <c r="W31" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="X31" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="X31" s="1" t="s">
+      <c r="Y31" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="Y31" s="1" t="s">
+      <c r="Z31" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="Z31" s="1" t="s">
+      <c r="AA31" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AA31" s="1" t="s">
+      <c r="AB31" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AB31" s="1" t="s">
+      <c r="AC31" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="AC31" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD31" s="1" t="s">
         <v>0</v>
       </c>
@@ -5525,6 +5614,9 @@
         <v>0</v>
       </c>
       <c r="AM31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5545,77 +5637,77 @@
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="S32" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="U32" s="1" t="s">
+      <c r="V32" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="V32" s="1" t="s">
+      <c r="W32" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="W32" s="1" t="s">
+      <c r="X32" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="X32" s="1" t="s">
+      <c r="Y32" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Y32" s="1" t="s">
+      <c r="Z32" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="Z32" s="1" t="s">
+      <c r="AA32" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AA32" s="1" t="s">
+      <c r="AB32" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="AB32" s="1" t="s">
+      <c r="AC32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="AC32" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD32" s="1" t="s">
         <v>0</v>
       </c>
@@ -5644,6 +5736,9 @@
         <v>0</v>
       </c>
       <c r="AM32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5664,77 +5759,77 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="R33" s="1" t="s">
+      <c r="S33" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="T33" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="T33" s="1" t="s">
+      <c r="U33" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="U33" s="1" t="s">
+      <c r="V33" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="V33" s="1" t="s">
+      <c r="W33" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="W33" s="1" t="s">
+      <c r="X33" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="X33" s="1" t="s">
+      <c r="Y33" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="Y33" s="1" t="s">
+      <c r="Z33" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Z33" s="1" t="s">
+      <c r="AA33" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AA33" s="1" t="s">
+      <c r="AB33" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AB33" s="1" t="s">
+      <c r="AC33" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AC33" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD33" s="1" t="s">
         <v>0</v>
       </c>
@@ -5763,6 +5858,9 @@
         <v>0</v>
       </c>
       <c r="AM33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5783,77 +5881,77 @@
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="T34" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="U34" s="1" t="s">
+      <c r="V34" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="V34" s="1" t="s">
+      <c r="W34" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="W34" s="1" t="s">
+      <c r="X34" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="X34" s="1" t="s">
+      <c r="Y34" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="Y34" s="1" t="s">
+      <c r="Z34" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="Z34" s="1" t="s">
+      <c r="AA34" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="AA34" s="1" t="s">
+      <c r="AB34" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="AB34" s="1" t="s">
+      <c r="AC34" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="AC34" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD34" s="1" t="s">
         <v>0</v>
       </c>
@@ -5882,6 +5980,9 @@
         <v>0</v>
       </c>
       <c r="AM34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5902,77 +6003,77 @@
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="U35" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="V35" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="V35" s="1" t="s">
+      <c r="W35" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="W35" s="1" t="s">
+      <c r="X35" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="X35" s="1" t="s">
+      <c r="Y35" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="Y35" s="1" t="s">
+      <c r="Z35" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="Z35" s="1" t="s">
+      <c r="AA35" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="AA35" s="1" t="s">
+      <c r="AB35" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="AB35" s="1" t="s">
+      <c r="AC35" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="AC35" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD35" s="1" t="s">
         <v>0</v>
       </c>
@@ -6001,6 +6102,9 @@
         <v>0</v>
       </c>
       <c r="AM35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN35" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6021,77 +6125,77 @@
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="P36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="R36" s="1" t="s">
+      <c r="S36" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="U36" s="1" t="s">
+      <c r="V36" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="V36" s="1" t="s">
+      <c r="W36" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="W36" s="1" t="s">
+      <c r="X36" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="X36" s="1" t="s">
+      <c r="Y36" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="Y36" s="1" t="s">
+      <c r="Z36" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="Z36" s="1" t="s">
+      <c r="AA36" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="AA36" s="1" t="s">
+      <c r="AB36" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="AB36" s="1" t="s">
+      <c r="AC36" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="AC36" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD36" s="1" t="s">
         <v>0</v>
       </c>
@@ -6120,6 +6224,9 @@
         <v>0</v>
       </c>
       <c r="AM36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN36" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6140,77 +6247,77 @@
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="P37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="R37" s="1" t="s">
+      <c r="S37" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="U37" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="U37" s="1" t="s">
+      <c r="V37" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="V37" s="1" t="s">
+      <c r="W37" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="W37" s="1" t="s">
+      <c r="X37" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="X37" s="1" t="s">
+      <c r="Y37" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="Y37" s="1" t="s">
+      <c r="Z37" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="Z37" s="1" t="s">
+      <c r="AA37" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="AA37" s="1" t="s">
+      <c r="AB37" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="AB37" s="1" t="s">
+      <c r="AC37" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="AC37" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD37" s="1" t="s">
         <v>0</v>
       </c>
@@ -6239,6 +6346,9 @@
         <v>0</v>
       </c>
       <c r="AM37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6259,77 +6369,77 @@
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="O38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="P38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="R38" s="1" t="s">
+      <c r="S38" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="U38" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="U38" s="1" t="s">
+      <c r="V38" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="V38" s="1" t="s">
+      <c r="W38" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="W38" s="1" t="s">
+      <c r="X38" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="X38" s="1" t="s">
+      <c r="Y38" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="Y38" s="1" t="s">
+      <c r="Z38" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="Z38" s="1" t="s">
+      <c r="AA38" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="AA38" s="1" t="s">
+      <c r="AB38" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="AB38" s="1" t="s">
+      <c r="AC38" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="AC38" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD38" s="1" t="s">
         <v>0</v>
       </c>
@@ -6358,6 +6468,9 @@
         <v>0</v>
       </c>
       <c r="AM38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6378,77 +6491,77 @@
         <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="R39" s="1" t="s">
+      <c r="S39" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="T39" s="1" t="s">
+      <c r="U39" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="U39" s="1" t="s">
+      <c r="V39" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="V39" s="1" t="s">
+      <c r="W39" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="W39" s="1" t="s">
+      <c r="X39" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="X39" s="1" t="s">
+      <c r="Y39" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="Y39" s="1" t="s">
+      <c r="Z39" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="Z39" s="1" t="s">
+      <c r="AA39" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="AA39" s="1" t="s">
+      <c r="AB39" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="AB39" s="1" t="s">
+      <c r="AC39" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="AC39" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD39" s="1" t="s">
         <v>0</v>
       </c>
@@ -6477,6 +6590,9 @@
         <v>0</v>
       </c>
       <c r="AM39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6512,62 +6628,62 @@
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="R40" s="1" t="s">
+      <c r="S40" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="T40" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="V40" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="V40" s="1" t="s">
+      <c r="W40" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="W40" s="1" t="s">
+      <c r="X40" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="X40" s="1" t="s">
+      <c r="Y40" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="Y40" s="1" t="s">
+      <c r="Z40" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="Z40" s="1" t="s">
+      <c r="AA40" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="AA40" s="1" t="s">
+      <c r="AB40" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="AB40" s="1" t="s">
+      <c r="AC40" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="AC40" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD40" s="1" t="s">
         <v>0</v>
       </c>
@@ -6596,6 +6712,9 @@
         <v>0</v>
       </c>
       <c r="AM40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6631,62 +6750,62 @@
         <v>0</v>
       </c>
       <c r="K41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="O41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="Q41" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="Q41" s="1" t="s">
+      <c r="R41" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="R41" s="1" t="s">
+      <c r="S41" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="U41" s="1" t="s">
+      <c r="V41" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="V41" s="1" t="s">
+      <c r="W41" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="W41" s="1" t="s">
+      <c r="X41" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="X41" s="1" t="s">
+      <c r="Y41" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="Y41" s="1" t="s">
+      <c r="Z41" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="Z41" s="1" t="s">
+      <c r="AA41" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="AA41" s="1" t="s">
+      <c r="AB41" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="AB41" s="1" t="s">
+      <c r="AC41" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="AC41" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD41" s="1" t="s">
         <v>0</v>
       </c>
@@ -6715,6 +6834,9 @@
         <v>0</v>
       </c>
       <c r="AM41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6750,62 +6872,62 @@
         <v>0</v>
       </c>
       <c r="K42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="O42" s="1" t="s">
+      <c r="P42" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="P42" s="1" t="s">
+      <c r="Q42" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="R42" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="R42" s="1" t="s">
+      <c r="S42" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="U42" s="1" t="s">
+      <c r="V42" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="V42" s="1" t="s">
+      <c r="W42" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="W42" s="1" t="s">
+      <c r="X42" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="X42" s="1" t="s">
+      <c r="Y42" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="Y42" s="1" t="s">
+      <c r="Z42" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="Z42" s="1" t="s">
+      <c r="AA42" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="AA42" s="1" t="s">
+      <c r="AB42" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="AB42" s="1" t="s">
+      <c r="AC42" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="AC42" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD42" s="1" t="s">
         <v>0</v>
       </c>
@@ -6834,6 +6956,9 @@
         <v>0</v>
       </c>
       <c r="AM42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN42" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6869,62 +6994,62 @@
         <v>0</v>
       </c>
       <c r="K43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="O43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="P43" s="1" t="s">
+      <c r="Q43" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="R43" s="1" t="s">
+      <c r="S43" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="U43" s="1" t="s">
+      <c r="V43" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="V43" s="1" t="s">
+      <c r="W43" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="W43" s="1" t="s">
+      <c r="X43" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="X43" s="1" t="s">
+      <c r="Y43" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="Y43" s="1" t="s">
+      <c r="Z43" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="Z43" s="1" t="s">
+      <c r="AA43" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="AA43" s="1" t="s">
+      <c r="AB43" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="AB43" s="1" t="s">
+      <c r="AC43" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="AC43" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD43" s="1" t="s">
         <v>0</v>
       </c>
@@ -6953,6 +7078,9 @@
         <v>0</v>
       </c>
       <c r="AM43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN43" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6988,62 +7116,62 @@
         <v>0</v>
       </c>
       <c r="K44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="O44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="P44" s="1" t="s">
+      <c r="Q44" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="R44" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="R44" s="1" t="s">
+      <c r="S44" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="U44" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="U44" s="1" t="s">
+      <c r="V44" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="V44" s="1" t="s">
+      <c r="W44" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="W44" s="1" t="s">
+      <c r="X44" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="X44" s="1" t="s">
+      <c r="Y44" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="Y44" s="1" t="s">
+      <c r="Z44" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="Z44" s="1" t="s">
+      <c r="AA44" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="AA44" s="1" t="s">
+      <c r="AB44" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="AB44" s="1" t="s">
+      <c r="AC44" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="AC44" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD44" s="1" t="s">
         <v>0</v>
       </c>
@@ -7072,6 +7200,9 @@
         <v>0</v>
       </c>
       <c r="AM44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN44" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7107,62 +7238,62 @@
         <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="O45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="Q45" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="R45" s="1" t="s">
+      <c r="S45" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="T45" s="1" t="s">
+      <c r="U45" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="U45" s="1" t="s">
+      <c r="V45" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="V45" s="1" t="s">
+      <c r="W45" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="W45" s="1" t="s">
+      <c r="X45" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="X45" s="1" t="s">
+      <c r="Y45" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="Y45" s="1" t="s">
+      <c r="Z45" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="Z45" s="1" t="s">
+      <c r="AA45" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="AA45" s="1" t="s">
+      <c r="AB45" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="AB45" s="1" t="s">
+      <c r="AC45" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="AC45" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD45" s="1" t="s">
         <v>0</v>
       </c>
@@ -7191,6 +7322,9 @@
         <v>0</v>
       </c>
       <c r="AM45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN45" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7226,62 +7360,62 @@
         <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="O46" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="Q46" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="R46" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="R46" s="1" t="s">
+      <c r="S46" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="U46" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="U46" s="1" t="s">
+      <c r="V46" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="V46" s="1" t="s">
+      <c r="W46" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="W46" s="1" t="s">
+      <c r="X46" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="X46" s="1" t="s">
+      <c r="Y46" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="Y46" s="1" t="s">
+      <c r="Z46" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="Z46" s="1" t="s">
+      <c r="AA46" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="AA46" s="1" t="s">
+      <c r="AB46" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="AB46" s="1" t="s">
+      <c r="AC46" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="AC46" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD46" s="1" t="s">
         <v>0</v>
       </c>
@@ -7310,6 +7444,9 @@
         <v>0</v>
       </c>
       <c r="AM46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7345,62 +7482,62 @@
         <v>0</v>
       </c>
       <c r="K47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="O47" s="1" t="s">
+      <c r="P47" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="P47" s="1" t="s">
+      <c r="Q47" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="Q47" s="1" t="s">
+      <c r="R47" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="R47" s="1" t="s">
+      <c r="S47" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="U47" s="1" t="s">
+      <c r="V47" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="V47" s="1" t="s">
+      <c r="W47" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="W47" s="1" t="s">
+      <c r="X47" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="X47" s="1" t="s">
+      <c r="Y47" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="Y47" s="1" t="s">
+      <c r="Z47" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="Z47" s="1" t="s">
+      <c r="AA47" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="AA47" s="1" t="s">
+      <c r="AB47" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="AB47" s="1" t="s">
+      <c r="AC47" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="AC47" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD47" s="1" t="s">
         <v>0</v>
       </c>
@@ -7429,6 +7566,9 @@
         <v>0</v>
       </c>
       <c r="AM47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN47" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7497,29 +7637,29 @@
         <v>0</v>
       </c>
       <c r="V48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W48" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="W48" s="1" t="s">
+      <c r="X48" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="X48" s="1" t="s">
+      <c r="Y48" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="Y48" s="1" t="s">
+      <c r="Z48" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="Z48" s="1" t="s">
+      <c r="AA48" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="AA48" s="1" t="s">
+      <c r="AB48" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="AB48" s="1" t="s">
+      <c r="AC48" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="AC48" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="AD48" s="1" t="s">
         <v>0</v>
       </c>
@@ -7548,6 +7688,9 @@
         <v>0</v>
       </c>
       <c r="AM48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN48" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7669,6 +7812,9 @@
       <c r="AM49" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN49" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -7788,6 +7934,9 @@
       <c r="AM50" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN50" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -7907,6 +8056,9 @@
       <c r="AM51" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN51" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -8026,6 +8178,9 @@
       <c r="AM52" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN52" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -8143,6 +8298,9 @@
         <v>0</v>
       </c>
       <c r="AM53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN53" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>